<commit_message>
fix: MysteryBox 확률 수정
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MysteryBoxTable.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MysteryBoxTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D3B2A3-5599-466F-AAED-3A15948C52D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF383E68-33CA-49DF-BB5E-B2C1E615C8BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12180" xr2:uid="{6502EAC7-2D35-4967-860C-E3330915121A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>key</t>
   </si>
@@ -45,25 +45,6 @@
   </si>
   <si>
     <t>이름</t>
-  </si>
-  <si>
-    <t>Kolibri</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>M1911</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DGL-50</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X18</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASVal</t>
   </si>
   <si>
     <t>MX16A4</t>
@@ -529,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB163613-AEB8-425E-BCE5-6CE1C560E9D3}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -552,16 +533,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -592,113 +573,113 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>10101</v>
+        <v>10202</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
-        <v>4</v>
+      <c r="C4" s="5">
+        <v>9</v>
       </c>
       <c r="D4" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>10102</v>
+        <v>10203</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
-        <v>4</v>
+      <c r="C5" s="5">
+        <v>9</v>
       </c>
       <c r="D5" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>10103</v>
+        <v>10204</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
-        <v>5</v>
+      <c r="C6" s="5">
+        <v>9</v>
       </c>
       <c r="D6" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>10104</v>
+        <v>10205</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F7" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>10201</v>
+        <v>10206</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5">
         <v>10</v>
@@ -706,39 +687,39 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>10202</v>
+        <v>10207</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>10203</v>
+        <v>10303</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5">
         <v>8</v>
-      </c>
-      <c r="D10" s="4">
-        <v>7</v>
-      </c>
-      <c r="E10" s="5">
-        <v>7</v>
       </c>
       <c r="F10" s="5">
         <v>8</v>
@@ -746,93 +727,93 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>10204</v>
+        <v>10304</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4">
         <v>7</v>
       </c>
       <c r="E11" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>10205</v>
+        <v>10401</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
         <v>8</v>
       </c>
-      <c r="D12" s="4">
-        <v>6</v>
-      </c>
       <c r="E12" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10206</v>
+        <v>10402</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5">
         <v>6</v>
       </c>
       <c r="F13" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>10207</v>
+        <v>10501</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="5">
-        <v>8</v>
+      <c r="C14" s="4">
+        <v>7</v>
       </c>
       <c r="D14" s="4">
         <v>6</v>
       </c>
       <c r="E14" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>10303</v>
+        <v>10601</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5">
-        <v>5</v>
+      <c r="C15" s="4">
+        <v>7</v>
       </c>
       <c r="D15" s="4">
         <v>6</v>
@@ -841,111 +822,12 @@
         <v>5</v>
       </c>
       <c r="F15" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>10304</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="5">
         <v>5</v>
-      </c>
-      <c r="D16" s="4">
-        <v>4</v>
-      </c>
-      <c r="E16" s="5">
-        <v>5</v>
-      </c>
-      <c r="F16" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>10401</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="5">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>10402</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4">
-        <v>4</v>
-      </c>
-      <c r="E18" s="5">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>10501</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4">
-        <v>3</v>
-      </c>
-      <c r="E19" s="5">
-        <v>3</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>10601</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5">
-        <v>3</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: mystery box 확률 변경
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MysteryBoxTable.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/MysteryBoxTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF383E68-33CA-49DF-BB5E-B2C1E615C8BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472CC9D9-52B3-415A-919C-E4C76E7AF67F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12180" xr2:uid="{6502EAC7-2D35-4967-860C-E3330915121A}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -593,16 +593,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F4" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -613,16 +613,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -633,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F6" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -653,16 +653,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F7" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -673,16 +673,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -693,16 +693,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -713,16 +713,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,16 +733,16 @@
         <v>13</v>
       </c>
       <c r="C11" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,16 +753,16 @@
         <v>14</v>
       </c>
       <c r="C12" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,16 +773,16 @@
         <v>15</v>
       </c>
       <c r="C13" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -793,16 +793,16 @@
         <v>16</v>
       </c>
       <c r="C14" s="4">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D14" s="4">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F14" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -813,16 +813,16 @@
         <v>17</v>
       </c>
       <c r="C15" s="4">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D15" s="4">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F15" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>